<commit_message>
Updated results excel file
</commit_message>
<xml_diff>
--- a/Results_and_scripts_ps/Benchmark_filenames.xlsx
+++ b/Results_and_scripts_ps/Benchmark_filenames.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="52">
   <si>
     <t>10 sections</t>
   </si>
@@ -160,6 +160,18 @@
   </si>
   <si>
     <t>run_20130613T172406</t>
+  </si>
+  <si>
+    <t>90 sections</t>
+  </si>
+  <si>
+    <t>run_20130613T182757</t>
+  </si>
+  <si>
+    <t>120 sections</t>
+  </si>
+  <si>
+    <t>run_20130613T224949</t>
   </si>
 </sst>
 </file>
@@ -400,11 +412,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="37731712"/>
-        <c:axId val="106480768"/>
+        <c:axId val="91957888"/>
+        <c:axId val="119370112"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="37731712"/>
+        <c:axId val="91957888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -414,12 +426,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106480768"/>
+        <c:crossAx val="119370112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="106480768"/>
+        <c:axId val="119370112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -430,14 +442,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="37731712"/>
+        <c:crossAx val="91957888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -550,11 +561,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="114917760"/>
-        <c:axId val="106489728"/>
+        <c:axId val="129053824"/>
+        <c:axId val="129055360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="114917760"/>
+        <c:axId val="129053824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -564,12 +575,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106489728"/>
+        <c:crossAx val="129055360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="106489728"/>
+        <c:axId val="129055360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -580,7 +591,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114917760"/>
+        <c:crossAx val="129053824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3088,10 +3099,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="I4:V51"/>
+  <dimension ref="I4:V75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F4" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView tabSelected="1" topLeftCell="E40" workbookViewId="0">
+      <selection activeCell="I68" sqref="I68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4124,11 +4135,9 @@
       <c r="Q47">
         <v>93.590489064637197</v>
       </c>
-      <c r="R47" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="S47" t="s">
-        <v>46</v>
+      <c r="R47" s="8">
+        <f t="shared" si="3"/>
+        <v>10.398943229404132</v>
       </c>
     </row>
     <row r="48" spans="9:19" x14ac:dyDescent="0.25">
@@ -4158,7 +4167,7 @@
         <v>6.1789059594969888</v>
       </c>
     </row>
-    <row r="49" spans="10:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="9:19" x14ac:dyDescent="0.25">
       <c r="K49">
         <v>7</v>
       </c>
@@ -4185,7 +4194,7 @@
         <v>17.023808055167553</v>
       </c>
     </row>
-    <row r="50" spans="10:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="9:19" x14ac:dyDescent="0.25">
       <c r="K50">
         <v>8</v>
       </c>
@@ -4212,7 +4221,7 @@
         <v>16.689812066519998</v>
       </c>
     </row>
-    <row r="51" spans="10:18" x14ac:dyDescent="0.25">
+    <row r="51" spans="9:19" x14ac:dyDescent="0.25">
       <c r="J51" s="3" t="s">
         <v>28</v>
       </c>
@@ -4228,7 +4237,551 @@
       </c>
       <c r="R51" s="3">
         <f>AVERAGE(R43:R50)</f>
-        <v>11.996514670880259</v>
+        <v>11.796818240695742</v>
+      </c>
+    </row>
+    <row r="54" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="K54" t="s">
+        <v>1</v>
+      </c>
+      <c r="L54" t="s">
+        <v>13</v>
+      </c>
+      <c r="M54" t="s">
+        <v>14</v>
+      </c>
+      <c r="N54" t="s">
+        <v>15</v>
+      </c>
+      <c r="O54" t="s">
+        <v>16</v>
+      </c>
+      <c r="P54" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>27</v>
+      </c>
+      <c r="R54" t="s">
+        <v>33</v>
+      </c>
+      <c r="S54" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="55" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I55" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J55" s="2"/>
+      <c r="K55">
+        <v>1</v>
+      </c>
+      <c r="L55" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M55" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N55" s="2">
+        <v>0</v>
+      </c>
+      <c r="O55" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="P55" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q55">
+        <v>273.90714073817497</v>
+      </c>
+      <c r="R55" s="8">
+        <f t="shared" ref="R55:R62" si="4">Q55/9</f>
+        <v>30.434126748686108</v>
+      </c>
+    </row>
+    <row r="56" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I56" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="J56" s="8"/>
+      <c r="K56">
+        <v>2</v>
+      </c>
+      <c r="L56" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M56" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N56" s="2">
+        <v>1</v>
+      </c>
+      <c r="O56" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="P56" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q56">
+        <v>276.27557210412101</v>
+      </c>
+      <c r="R56" s="8">
+        <f t="shared" si="4"/>
+        <v>30.697285789346779</v>
+      </c>
+    </row>
+    <row r="57" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="K57">
+        <v>3</v>
+      </c>
+      <c r="L57" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M57" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N57" s="2">
+        <v>0</v>
+      </c>
+      <c r="O57" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="P57" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q57">
+        <v>663.08986961590301</v>
+      </c>
+      <c r="R57" s="8">
+        <f t="shared" si="4"/>
+        <v>73.676652179544774</v>
+      </c>
+    </row>
+    <row r="58" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="K58">
+        <v>4</v>
+      </c>
+      <c r="L58" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M58" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N58" s="2">
+        <v>1</v>
+      </c>
+      <c r="O58" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="P58" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q58">
+        <v>680.77073597821698</v>
+      </c>
+      <c r="R58" s="8">
+        <f t="shared" si="4"/>
+        <v>75.641192886468559</v>
+      </c>
+    </row>
+    <row r="59" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="K59">
+        <v>5</v>
+      </c>
+      <c r="L59" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M59" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N59" s="2">
+        <v>0</v>
+      </c>
+      <c r="O59" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="P59" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q59">
+        <v>253.40281325617099</v>
+      </c>
+      <c r="R59" s="8">
+        <f t="shared" si="4"/>
+        <v>28.155868139574554</v>
+      </c>
+    </row>
+    <row r="60" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="K60">
+        <v>6</v>
+      </c>
+      <c r="L60" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M60" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N60" s="2">
+        <v>1</v>
+      </c>
+      <c r="O60" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="P60" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q60">
+        <v>259.19635707058302</v>
+      </c>
+      <c r="R60" s="8">
+        <f t="shared" si="4"/>
+        <v>28.799595230064782</v>
+      </c>
+    </row>
+    <row r="61" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="K61">
+        <v>7</v>
+      </c>
+      <c r="L61" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M61" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N61" s="2">
+        <v>0</v>
+      </c>
+      <c r="O61" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="P61" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q61">
+        <v>721.93327047443995</v>
+      </c>
+      <c r="R61" s="8">
+        <f t="shared" si="4"/>
+        <v>80.214807830493328</v>
+      </c>
+    </row>
+    <row r="62" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="K62">
+        <v>8</v>
+      </c>
+      <c r="L62" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M62" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N62" s="2">
+        <v>1</v>
+      </c>
+      <c r="O62" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="P62" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q62">
+        <v>688.41997373396305</v>
+      </c>
+      <c r="R62" s="8">
+        <f t="shared" si="4"/>
+        <v>76.491108192662566</v>
+      </c>
+    </row>
+    <row r="63" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="J63" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K63" s="3"/>
+      <c r="L63" s="3"/>
+      <c r="M63" s="3"/>
+      <c r="N63" s="3"/>
+      <c r="O63" s="3"/>
+      <c r="P63" s="3"/>
+      <c r="Q63" s="5">
+        <f>AVERAGE(Q55:Q62)</f>
+        <v>477.12446662144669</v>
+      </c>
+      <c r="R63" s="3">
+        <f>AVERAGE(R55:R62)</f>
+        <v>53.013829624605187</v>
+      </c>
+    </row>
+    <row r="66" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="K66" t="s">
+        <v>1</v>
+      </c>
+      <c r="L66" t="s">
+        <v>13</v>
+      </c>
+      <c r="M66" t="s">
+        <v>14</v>
+      </c>
+      <c r="N66" t="s">
+        <v>15</v>
+      </c>
+      <c r="O66" t="s">
+        <v>16</v>
+      </c>
+      <c r="P66" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q66" t="s">
+        <v>27</v>
+      </c>
+      <c r="R66" t="s">
+        <v>33</v>
+      </c>
+      <c r="S66" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="67" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I67" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="J67" s="2"/>
+      <c r="K67">
+        <v>1</v>
+      </c>
+      <c r="L67" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M67" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N67" s="2">
+        <v>0</v>
+      </c>
+      <c r="O67" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="P67" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q67">
+        <v>273.90714073817497</v>
+      </c>
+      <c r="R67" s="8">
+        <f t="shared" ref="R67:R74" si="5">Q67/9</f>
+        <v>30.434126748686108</v>
+      </c>
+    </row>
+    <row r="68" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I68" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="J68" s="8"/>
+      <c r="K68">
+        <v>2</v>
+      </c>
+      <c r="L68" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M68" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N68" s="2">
+        <v>1</v>
+      </c>
+      <c r="O68" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="P68" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q68">
+        <v>276.27557210412101</v>
+      </c>
+      <c r="R68" s="8">
+        <f t="shared" si="5"/>
+        <v>30.697285789346779</v>
+      </c>
+    </row>
+    <row r="69" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="K69">
+        <v>3</v>
+      </c>
+      <c r="L69" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M69" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N69" s="2">
+        <v>0</v>
+      </c>
+      <c r="O69" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="P69" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q69">
+        <v>663.08986961590301</v>
+      </c>
+      <c r="R69" s="8">
+        <f t="shared" si="5"/>
+        <v>73.676652179544774</v>
+      </c>
+    </row>
+    <row r="70" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="K70">
+        <v>4</v>
+      </c>
+      <c r="L70" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M70" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N70" s="2">
+        <v>1</v>
+      </c>
+      <c r="O70" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="P70" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q70">
+        <v>680.77073597821698</v>
+      </c>
+      <c r="R70" s="8">
+        <f t="shared" si="5"/>
+        <v>75.641192886468559</v>
+      </c>
+    </row>
+    <row r="71" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="K71">
+        <v>5</v>
+      </c>
+      <c r="L71" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M71" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N71" s="2">
+        <v>0</v>
+      </c>
+      <c r="O71" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="P71" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q71">
+        <v>253.40281325617099</v>
+      </c>
+      <c r="R71" s="8">
+        <f t="shared" si="5"/>
+        <v>28.155868139574554</v>
+      </c>
+    </row>
+    <row r="72" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="K72">
+        <v>6</v>
+      </c>
+      <c r="L72" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M72" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N72" s="2">
+        <v>1</v>
+      </c>
+      <c r="O72" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="P72" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q72">
+        <v>259.19635707058302</v>
+      </c>
+      <c r="R72" s="8">
+        <f t="shared" si="5"/>
+        <v>28.799595230064782</v>
+      </c>
+    </row>
+    <row r="73" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="K73">
+        <v>7</v>
+      </c>
+      <c r="L73" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M73" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N73" s="2">
+        <v>0</v>
+      </c>
+      <c r="O73" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="P73" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q73">
+        <v>721.93327047443995</v>
+      </c>
+      <c r="R73" s="8">
+        <f t="shared" si="5"/>
+        <v>80.214807830493328</v>
+      </c>
+    </row>
+    <row r="74" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="K74">
+        <v>8</v>
+      </c>
+      <c r="L74" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M74" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N74" s="2">
+        <v>1</v>
+      </c>
+      <c r="O74" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="P74" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q74">
+        <v>688.41997373396305</v>
+      </c>
+      <c r="R74" s="8">
+        <f t="shared" si="5"/>
+        <v>76.491108192662566</v>
+      </c>
+    </row>
+    <row r="75" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="J75" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K75" s="3"/>
+      <c r="L75" s="3"/>
+      <c r="M75" s="3"/>
+      <c r="N75" s="3"/>
+      <c r="O75" s="3"/>
+      <c r="P75" s="3"/>
+      <c r="Q75" s="5">
+        <f>AVERAGE(Q67:Q74)</f>
+        <v>477.12446662144669</v>
+      </c>
+      <c r="R75" s="3">
+        <f>AVERAGE(R67:R74)</f>
+        <v>53.013829624605187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated benchmark excel file
</commit_message>
<xml_diff>
--- a/Results_and_scripts_ps/Benchmark_filenames.xlsx
+++ b/Results_and_scripts_ps/Benchmark_filenames.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="28620" windowHeight="12660" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="28620" windowHeight="12660" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="55">
   <si>
     <t>10 sections</t>
   </si>
@@ -172,6 +172,15 @@
   </si>
   <si>
     <t>run_20130613T224949</t>
+  </si>
+  <si>
+    <t>200 sections</t>
+  </si>
+  <si>
+    <t>run_20130615T044607</t>
+  </si>
+  <si>
+    <t>Parametrit</t>
   </si>
 </sst>
 </file>
@@ -412,11 +421,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="91957888"/>
-        <c:axId val="119370112"/>
+        <c:axId val="38972800"/>
+        <c:axId val="105694336"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="91957888"/>
+        <c:axId val="38972800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -426,12 +435,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="119370112"/>
+        <c:crossAx val="105694336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="119370112"/>
+        <c:axId val="105694336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -442,7 +451,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91957888"/>
+        <c:crossAx val="38972800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -492,7 +501,8 @@
             </a:ln>
           </c:spPr>
           <c:trendline>
-            <c:trendlineType val="exp"/>
+            <c:trendlineType val="poly"/>
+            <c:order val="3"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -548,6 +558,15 @@
                 <c:pt idx="3">
                   <c:v>11.996514670880259</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>53.013829624605187</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>217.90809646327875</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1569.7912974591188</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -561,11 +580,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="129053824"/>
-        <c:axId val="129055360"/>
+        <c:axId val="106030976"/>
+        <c:axId val="106032512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="129053824"/>
+        <c:axId val="106030976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -575,14 +594,15 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="129055360"/>
+        <c:crossAx val="106032512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="129055360"/>
+        <c:axId val="106032512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -591,7 +611,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="129053824"/>
+        <c:crossAx val="106030976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -600,6 +620,178 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="fi-FI"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="poly"/>
+            <c:order val="3"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.2722222222222222E-2"/>
+                  <c:y val="1.1630941965587635E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$U$5:$U$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$V$5:$V$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.1627141821457582</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.50271568502206931</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.3734660792200744</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.996514670880259</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>53.013829624605187</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>217.90809646327875</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1569.7912974591188</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="84306176"/>
+        <c:axId val="84328448"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="84306176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="200"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="84328448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="84328448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="84306176"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -662,6 +854,43 @@
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -3099,10 +3328,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="I4:V75"/>
+  <dimension ref="I4:V87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E40" workbookViewId="0">
-      <selection activeCell="I68" sqref="I68"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="U4" sqref="U4:V11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3264,6 +3493,9 @@
       <c r="U9">
         <v>90</v>
       </c>
+      <c r="V9">
+        <v>53.013829624605187</v>
+      </c>
     </row>
     <row r="10" spans="9:22" x14ac:dyDescent="0.25">
       <c r="K10">
@@ -3294,6 +3526,9 @@
       <c r="U10">
         <v>120</v>
       </c>
+      <c r="V10">
+        <v>217.90809646327875</v>
+      </c>
     </row>
     <row r="11" spans="9:22" x14ac:dyDescent="0.25">
       <c r="K11">
@@ -3323,6 +3558,9 @@
       </c>
       <c r="U11">
         <v>200</v>
+      </c>
+      <c r="V11">
+        <v>1569.7912974591188</v>
       </c>
     </row>
     <row r="12" spans="9:22" x14ac:dyDescent="0.25">
@@ -4565,11 +4803,11 @@
         <v>36</v>
       </c>
       <c r="Q67">
-        <v>273.90714073817497</v>
+        <v>1053.9804746167099</v>
       </c>
       <c r="R67" s="8">
         <f t="shared" ref="R67:R74" si="5">Q67/9</f>
-        <v>30.434126748686108</v>
+        <v>117.10894162407888</v>
       </c>
     </row>
     <row r="68" spans="9:19" x14ac:dyDescent="0.25">
@@ -4596,11 +4834,11 @@
         <v>36</v>
       </c>
       <c r="Q68">
-        <v>276.27557210412101</v>
+        <v>1083.1161154486999</v>
       </c>
       <c r="R68" s="8">
         <f t="shared" si="5"/>
-        <v>30.697285789346779</v>
+        <v>120.34623504985555</v>
       </c>
     </row>
     <row r="69" spans="9:19" x14ac:dyDescent="0.25">
@@ -4623,11 +4861,11 @@
         <v>37</v>
       </c>
       <c r="Q69">
-        <v>663.08986961590301</v>
+        <v>2780.7640684456401</v>
       </c>
       <c r="R69" s="8">
         <f t="shared" si="5"/>
-        <v>73.676652179544774</v>
+        <v>308.97378538284892</v>
       </c>
     </row>
     <row r="70" spans="9:19" x14ac:dyDescent="0.25">
@@ -4650,11 +4888,11 @@
         <v>37</v>
       </c>
       <c r="Q70">
-        <v>680.77073597821698</v>
+        <v>2697.6612027535998</v>
       </c>
       <c r="R70" s="8">
         <f t="shared" si="5"/>
-        <v>75.641192886468559</v>
+        <v>299.74013363928884</v>
       </c>
     </row>
     <row r="71" spans="9:19" x14ac:dyDescent="0.25">
@@ -4677,11 +4915,11 @@
         <v>36</v>
       </c>
       <c r="Q71">
-        <v>253.40281325617099</v>
+        <v>1117.8539909784699</v>
       </c>
       <c r="R71" s="8">
         <f t="shared" si="5"/>
-        <v>28.155868139574554</v>
+        <v>124.20599899760776</v>
       </c>
     </row>
     <row r="72" spans="9:19" x14ac:dyDescent="0.25">
@@ -4704,11 +4942,11 @@
         <v>36</v>
       </c>
       <c r="Q72">
-        <v>259.19635707058302</v>
+        <v>1326.2061976944301</v>
       </c>
       <c r="R72" s="8">
         <f t="shared" si="5"/>
-        <v>28.799595230064782</v>
+        <v>147.35624418827001</v>
       </c>
     </row>
     <row r="73" spans="9:19" x14ac:dyDescent="0.25">
@@ -4731,11 +4969,11 @@
         <v>37</v>
       </c>
       <c r="Q73">
-        <v>721.93327047443995</v>
+        <v>2799.8093541088401</v>
       </c>
       <c r="R73" s="8">
         <f t="shared" si="5"/>
-        <v>80.214807830493328</v>
+        <v>311.08992823431555</v>
       </c>
     </row>
     <row r="74" spans="9:19" x14ac:dyDescent="0.25">
@@ -4758,11 +4996,11 @@
         <v>37</v>
       </c>
       <c r="Q74">
-        <v>688.41997373396305</v>
+        <v>2829.9915413096801</v>
       </c>
       <c r="R74" s="8">
         <f t="shared" si="5"/>
-        <v>76.491108192662566</v>
+        <v>314.44350458996445</v>
       </c>
     </row>
     <row r="75" spans="9:19" x14ac:dyDescent="0.25">
@@ -4777,11 +5015,285 @@
       <c r="P75" s="3"/>
       <c r="Q75" s="5">
         <f>AVERAGE(Q67:Q74)</f>
-        <v>477.12446662144669</v>
+        <v>1961.1728681695088</v>
       </c>
       <c r="R75" s="3">
         <f>AVERAGE(R67:R74)</f>
-        <v>53.013829624605187</v>
+        <v>217.90809646327875</v>
+      </c>
+    </row>
+    <row r="78" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="K78" t="s">
+        <v>1</v>
+      </c>
+      <c r="L78" t="s">
+        <v>13</v>
+      </c>
+      <c r="M78" t="s">
+        <v>14</v>
+      </c>
+      <c r="N78" t="s">
+        <v>15</v>
+      </c>
+      <c r="O78" t="s">
+        <v>16</v>
+      </c>
+      <c r="P78" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q78" t="s">
+        <v>27</v>
+      </c>
+      <c r="R78" t="s">
+        <v>33</v>
+      </c>
+      <c r="S78" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="79" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I79" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J79" s="2"/>
+      <c r="K79">
+        <v>1</v>
+      </c>
+      <c r="L79" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M79" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N79" s="2">
+        <v>0</v>
+      </c>
+      <c r="O79" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="P79" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q79">
+        <v>8351.2175597600508</v>
+      </c>
+      <c r="R79" s="8">
+        <f t="shared" ref="R79:R86" si="6">Q79/9</f>
+        <v>927.91306219556122</v>
+      </c>
+    </row>
+    <row r="80" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I80" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="J80" s="8"/>
+      <c r="K80">
+        <v>2</v>
+      </c>
+      <c r="L80" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M80" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N80" s="2">
+        <v>1</v>
+      </c>
+      <c r="O80" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="P80" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q80">
+        <v>8371.4985107894408</v>
+      </c>
+      <c r="R80" s="8">
+        <f t="shared" si="6"/>
+        <v>930.16650119882672</v>
+      </c>
+    </row>
+    <row r="81" spans="10:19" x14ac:dyDescent="0.25">
+      <c r="K81">
+        <v>3</v>
+      </c>
+      <c r="L81" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M81" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N81" s="2">
+        <v>0</v>
+      </c>
+      <c r="O81" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="P81" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q81">
+        <v>19127.279406817299</v>
+      </c>
+      <c r="R81" s="8">
+        <f t="shared" si="6"/>
+        <v>2125.2532674241443</v>
+      </c>
+    </row>
+    <row r="82" spans="10:19" x14ac:dyDescent="0.25">
+      <c r="K82">
+        <v>4</v>
+      </c>
+      <c r="L82" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M82" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N82" s="2">
+        <v>1</v>
+      </c>
+      <c r="O82" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="P82" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q82">
+        <v>19522.7376795768</v>
+      </c>
+      <c r="R82" s="8">
+        <f t="shared" si="6"/>
+        <v>2169.1930755085332</v>
+      </c>
+    </row>
+    <row r="83" spans="10:19" x14ac:dyDescent="0.25">
+      <c r="K83">
+        <v>5</v>
+      </c>
+      <c r="L83" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M83" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N83" s="2">
+        <v>0</v>
+      </c>
+      <c r="O83" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="P83" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q83">
+        <v>8088.495672518</v>
+      </c>
+      <c r="R83" s="8">
+        <f t="shared" si="6"/>
+        <v>898.72174139088884</v>
+      </c>
+    </row>
+    <row r="84" spans="10:19" x14ac:dyDescent="0.25">
+      <c r="K84">
+        <v>6</v>
+      </c>
+      <c r="L84" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M84" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N84" s="2">
+        <v>1</v>
+      </c>
+      <c r="O84" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="P84" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q84" t="s">
+        <v>44</v>
+      </c>
+      <c r="R84" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S84" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="85" spans="10:19" x14ac:dyDescent="0.25">
+      <c r="K85">
+        <v>7</v>
+      </c>
+      <c r="L85" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M85" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N85" s="2">
+        <v>0</v>
+      </c>
+      <c r="O85" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="P85" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q85">
+        <v>17976.227398138901</v>
+      </c>
+      <c r="R85" s="8">
+        <f t="shared" si="6"/>
+        <v>1997.3585997932112</v>
+      </c>
+    </row>
+    <row r="86" spans="10:19" x14ac:dyDescent="0.25">
+      <c r="K86">
+        <v>8</v>
+      </c>
+      <c r="L86" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M86" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N86" s="2">
+        <v>1</v>
+      </c>
+      <c r="O86" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="P86" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q86">
+        <v>17459.395512324001</v>
+      </c>
+      <c r="R86" s="8">
+        <f t="shared" si="6"/>
+        <v>1939.9328347026667</v>
+      </c>
+    </row>
+    <row r="87" spans="10:19" x14ac:dyDescent="0.25">
+      <c r="J87" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K87" s="3"/>
+      <c r="L87" s="3"/>
+      <c r="M87" s="3"/>
+      <c r="N87" s="3"/>
+      <c r="O87" s="3"/>
+      <c r="P87" s="3"/>
+      <c r="Q87" s="5">
+        <f>AVERAGE(Q79:Q86)</f>
+        <v>14128.121677132071</v>
+      </c>
+      <c r="R87" s="3">
+        <f>AVERAGE(R79:R86)</f>
+        <v>1569.7912974591188</v>
       </c>
     </row>
   </sheetData>
@@ -4793,12 +5305,252 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4">
+        <v>10</v>
+      </c>
+      <c r="I4">
+        <v>0.1627141821457582</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5">
+        <v>20</v>
+      </c>
+      <c r="I5">
+        <v>0.50271568502206931</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6">
+        <v>30</v>
+      </c>
+      <c r="I6">
+        <v>1.3734660792200744</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7">
+        <v>60</v>
+      </c>
+      <c r="I7">
+        <v>11.996514670880259</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8">
+        <v>90</v>
+      </c>
+      <c r="I8">
+        <v>53.013829624605187</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H9">
+        <v>120</v>
+      </c>
+      <c r="I9">
+        <v>217.90809646327875</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10">
+        <v>200</v>
+      </c>
+      <c r="I10">
+        <v>1569.7912974591188</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>